<commit_message>
semana 16 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -420,10 +420,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>0.37</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.14</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6">
@@ -501,10 +501,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -525,10 +525,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0.37</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="9">
@@ -546,10 +546,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -588,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -606,10 +606,10 @@
         </is>
       </c>
       <c r="C12">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D12">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E12">
         <v>0.05</v>
@@ -627,13 +627,13 @@
         </is>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="14">
@@ -648,13 +648,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -669,13 +669,13 @@
         </is>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -714,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -732,13 +732,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0.14</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>0.02</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="21">
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0.37</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="23">
@@ -840,10 +840,10 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <v>0.37</v>
@@ -892,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -934,10 +934,10 @@
         <v>5</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29">
@@ -952,13 +952,13 @@
         </is>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0.14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0.37</v>
@@ -1018,10 +1018,10 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
         <v>2</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
       <c r="E33">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="34">
@@ -1057,13 +1057,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="35">
@@ -1099,10 +1099,10 @@
         </is>
       </c>
       <c r="C36">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36">
         <v>0.1</v>

</xml_diff>

<commit_message>
semana 20 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -585,13 +585,13 @@
         </is>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="12">
@@ -651,10 +651,10 @@
         <v>3</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>0.15</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="15">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="17">
@@ -732,13 +732,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="19">
@@ -774,13 +774,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.05</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="21">
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>0.09</v>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>0.37</v>
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E27">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28">
@@ -931,13 +931,13 @@
         </is>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0.06</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="29">
@@ -955,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -976,10 +976,10 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -997,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1018,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>0.37</v>
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="34">
@@ -1057,13 +1057,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35">
@@ -1078,13 +1078,13 @@
         </is>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
       <c r="E35">
-        <v>0.13</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
semana 22 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.18</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="4">
@@ -438,13 +438,13 @@
         </is>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="5">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="6">
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -501,13 +501,13 @@
         </is>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="8">
@@ -555,19 +555,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>298</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Agresiones por animales potencialmente transmisores de rabia</t>
+          <t>Evento adverso grave posterior a la vacunacion</t>
         </is>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -576,138 +576,138 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>300</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hepatitis a</t>
+          <t>Agresiones por animales potencialmente transmisores de rabia</t>
         </is>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>330</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
+          <t>Hepatitis a</t>
         </is>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.06</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Enfermedades huerfanas - raras</t>
+          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
         </is>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0.01</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ira por virus nuevo</t>
+          <t>Enfermedades huerfanas - raras</t>
         </is>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Infeccion respiratoria aguda grave irag inusitada</t>
+          <t>Ira por virus nuevo</t>
         </is>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
+          <t>Infeccion respiratoria aguda grave irag inusitada</t>
         </is>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
+          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
         </is>
       </c>
       <c r="C17">
@@ -723,232 +723,232 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>355</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Intento de suicidio</t>
+          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
         </is>
       </c>
       <c r="C18">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.07000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>356</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Iad - infecciones asociadas a dispositivos - individual</t>
+          <t>Intento de suicidio</t>
         </is>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>0.37</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>357</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Intoxicaciones</t>
+          <t>Iad - infecciones asociadas a dispositivos - individual</t>
         </is>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.09</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>365</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Leishmaniasis cutanea</t>
+          <t>Intoxicaciones</t>
         </is>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>430</t>
-        </is>
+          <t>420</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Leishmaniasis cutanea</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>455</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Leptospirosis</t>
-        </is>
-      </c>
-      <c r="C23">
-        <v>1</v>
+          <t>430</t>
+        </is>
       </c>
       <c r="D23">
         <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0.37</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Malaria</t>
+          <t>Leptospirosis</t>
         </is>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>535</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
+          <t>Malaria</t>
         </is>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>535</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Morbilidad materna extrema</t>
+          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
         </is>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>549</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Mortalidad perinatal y neonatal tardia</t>
+          <t>Morbilidad materna extrema</t>
         </is>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>560</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Mortalidad por dengue</t>
+          <t>Mortalidad perinatal y neonatal tardia</t>
         </is>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>580</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
+          <t>Mortalidad por dengue</t>
         </is>
       </c>
       <c r="C29">
@@ -964,33 +964,33 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>591</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Parotiditis</t>
+          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
         </is>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>740</t>
+          <t>620</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sifilis congenita</t>
+          <t>Parotiditis</t>
         </is>
       </c>
       <c r="C31">
@@ -1006,105 +1006,126 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>740</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sifilis gestacional</t>
+          <t>Sifilis congenita</t>
         </is>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>0.27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>813</t>
+          <t>750</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tuberculosis</t>
+          <t>Sifilis gestacional</t>
         </is>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>0.01</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>831</t>
+          <t>813</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Varicela individual</t>
+          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C34">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>831</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Vih/sida/mortalidad por sida</t>
+          <t>Varicela individual</t>
         </is>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D35">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E35">
-        <v>0.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Vih/sida/mortalidad por sida</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>895</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>Zika</t>
         </is>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
semana 24 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0.37</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4">
@@ -438,13 +438,13 @@
         </is>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="5">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6">
@@ -483,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -501,13 +501,13 @@
         </is>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.18</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="8">
@@ -585,13 +585,13 @@
         </is>
       </c>
       <c r="C11">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -648,13 +648,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15">
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="17">
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="18">
@@ -735,10 +735,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C19">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0.07000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.14</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21">
@@ -798,10 +798,10 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22">
@@ -850,10 +850,10 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>0.37</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="25">
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E27">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28">
@@ -931,13 +931,13 @@
         </is>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1015,13 +1015,13 @@
         </is>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1036,10 +1036,10 @@
         </is>
       </c>
       <c r="C33">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1057,13 +1057,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="35">
@@ -1078,13 +1078,13 @@
         </is>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
semana 26 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,10 +420,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>0.37</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>0.18</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="6">
@@ -483,7 +483,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -501,13 +501,13 @@
         </is>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>0.14</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <v>20</v>
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="13">
@@ -648,13 +648,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>0.18</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0.14</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="17">
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C19">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.02</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="21">
@@ -798,10 +798,10 @@
         <v>6</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -847,13 +847,13 @@
         </is>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="25">
@@ -889,13 +889,13 @@
         </is>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="C27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="28">
@@ -985,103 +985,103 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>740</t>
+          <t>720</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sifilis congenita</t>
+          <t>Sindrome de rubeola congenita</t>
         </is>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>740</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sifilis gestacional</t>
+          <t>Sifilis congenita</t>
         </is>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>813</t>
+          <t>750</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tuberculosis</t>
+          <t>Sifilis gestacional</t>
         </is>
       </c>
       <c r="C33">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>831</t>
+          <t>813</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Varicela individual</t>
+          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C34">
         <v>7</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>850</t>
+          <t>831</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Vih/sida/mortalidad por sida</t>
+          <t>Varicela individual</t>
         </is>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1090,21 +1090,42 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Vih/sida/mortalidad por sida</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>895</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>Zika</t>
         </is>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
semana 28 y 29 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.22</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="4">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="6">
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -504,10 +504,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="8">
@@ -585,13 +585,13 @@
         </is>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D11">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -627,13 +627,13 @@
         </is>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.37</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="14">
@@ -669,10 +669,10 @@
         </is>
       </c>
       <c r="C15">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17">
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -732,13 +732,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="19">
@@ -753,10 +753,10 @@
         </is>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -774,13 +774,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.14</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="21">
@@ -795,13 +795,13 @@
         </is>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22">
@@ -847,13 +847,13 @@
         </is>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
         <v>2</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
       <c r="E24">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="25">
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E27">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="28">
@@ -931,13 +931,13 @@
         </is>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="29">
@@ -997,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1015,13 +1015,13 @@
         </is>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1039,10 +1039,10 @@
         <v>7</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1057,13 +1057,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1078,13 +1078,13 @@
         </is>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
semana 41 de 2024
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -399,10 +399,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="4">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="6">
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -504,10 +504,10 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>0.14</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="8">
@@ -585,13 +585,13 @@
         </is>
       </c>
       <c r="C11">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E11">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="13">
@@ -630,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.18</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="14">
@@ -648,13 +648,13 @@
         </is>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="15">
@@ -672,10 +672,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -732,13 +732,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -753,13 +753,13 @@
         </is>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         </is>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.37</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="21">
@@ -795,13 +795,13 @@
         </is>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22">
@@ -850,10 +850,10 @@
         <v>2</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0.27</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="25">
@@ -910,13 +910,13 @@
         </is>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>0.01</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="28">
@@ -931,13 +931,13 @@
         </is>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1046,13 +1046,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="35">
@@ -1067,13 +1067,13 @@
         </is>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="36">
@@ -1091,10 +1091,10 @@
         <v>10</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1109,13 +1109,13 @@
         </is>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E37">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="38">

</xml_diff>

<commit_message>
semana 04 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,208 +387,208 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>113</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Accidente ofidico</t>
+          <t>Desnutrici”n aguda en menores de 5 anos</t>
         </is>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Desnutrici”n aguda en menores de 5 anos</t>
+          <t>Cancer en menores de 18 anos</t>
         </is>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>155</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cancer en menores de 18 anos</t>
+          <t>Cancer de la mama y cuello uterino</t>
         </is>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>210</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cancer de la mama y cuello uterino</t>
+          <t>Dengue</t>
         </is>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="E5">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dengue</t>
+          <t>Defectos congenitos</t>
         </is>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>220</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Defectos congenitos</t>
+          <t>Dengue grave</t>
         </is>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>217</t>
+          <t>300</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Chikungunya</t>
+          <t>Agresiones por animales potencialmente transmisores de rabia</t>
         </is>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dengue grave</t>
+          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
         </is>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Evento adverso grave posterior a la vacunacion</t>
+          <t>Enfermedades huerfanas - raras</t>
         </is>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Agresiones por animales potencialmente transmisores de rabia</t>
+          <t>Ira por virus nuevo</t>
         </is>
       </c>
       <c r="C11">
-        <v>41</v>
+        <v>294</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -597,12 +597,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hepatitis a</t>
+          <t>Infeccion respiratoria aguda grave irag inusitada</t>
         </is>
       </c>
       <c r="C12">
@@ -618,40 +618,40 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>355</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
+          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
         </is>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>356</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Enfermedades huerfanas - raras</t>
+          <t>Intento de suicidio</t>
         </is>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>0.04</v>
@@ -660,431 +660,253 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>357</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Infeccion respiratoria aguda grave irag inusitada</t>
+          <t>Iad - infecciones asociadas a dispositivos - individual</t>
         </is>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.14</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>365</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
+          <t>Intoxicaciones</t>
         </is>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0.37</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
+          <t>Leptospirosis</t>
         </is>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Intento de suicidio</t>
+          <t>Malaria</t>
         </is>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>0.13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>549</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Iad - infecciones asociadas a dispositivos - individual</t>
+          <t>Morbilidad materna extrema</t>
         </is>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.37</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>560</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Intoxicaciones</t>
+          <t>Mortalidad perinatal y neonatal tardia</t>
         </is>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.09</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>620</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Leishmaniasis cutanea</t>
+          <t>Parotiditis</t>
         </is>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>430</t>
-        </is>
+          <t>740</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Sifilis congenita</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>750</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Leptospirosis</t>
+          <t>Sifilis gestacional</t>
         </is>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>813</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Malaria</t>
+          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>535</t>
+          <t>831</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
+          <t>Varicela individual</t>
         </is>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>850</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Morbilidad materna extrema</t>
+          <t>Vih/sida/mortalidad por sida</t>
         </is>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>560</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Mortalidad perinatal y neonatal tardia</t>
-        </is>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>580</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Mortalidad por dengue</t>
-        </is>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>620</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Parotiditis</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>740</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Sifilis congenita</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Sifilis gestacional</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>813</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
-        </is>
-      </c>
-      <c r="C32">
-        <v>6</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>831</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Varicela individual</t>
-        </is>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Vih/sida/mortalidad por sida</t>
-        </is>
-      </c>
-      <c r="C34">
-        <v>8</v>
-      </c>
-      <c r="D34">
-        <v>7</v>
-      </c>
-      <c r="E34">
-        <v>0.14</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>895</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Zika</t>
-        </is>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 22 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -396,13 +396,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
       <c r="E2">
-        <v>0.02</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="3">
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="4">
@@ -438,13 +438,13 @@
         </is>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="5">
@@ -459,10 +459,10 @@
         </is>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="7">
@@ -504,10 +504,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E8">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -567,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="11">
@@ -588,10 +588,10 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>0.02</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="12">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="C12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="13">
@@ -651,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0.37</v>
@@ -669,13 +669,13 @@
         </is>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="17">
@@ -732,13 +732,13 @@
         </is>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>0.03</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="19">
@@ -756,10 +756,10 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="20">
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -816,13 +816,13 @@
         </is>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="23">
@@ -837,13 +837,13 @@
         </is>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="24">
@@ -931,13 +931,13 @@
         </is>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -952,13 +952,13 @@
         </is>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0.14</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="30">
@@ -976,10 +976,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -994,13 +994,13 @@
         </is>
       </c>
       <c r="C31">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="32">
@@ -1015,13 +1015,13 @@
         </is>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="33">
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33">
         <v>9</v>
       </c>
-      <c r="D33">
-        <v>8</v>
-      </c>
       <c r="E33">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 30 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,10 +399,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -417,13 +417,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>0.04</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="4">
@@ -441,10 +441,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -501,13 +501,13 @@
         </is>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="8">
@@ -543,178 +543,167 @@
         </is>
       </c>
       <c r="C9">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>37</v>
       </c>
       <c r="E9">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>330</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Hepatitis a</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>0</v>
+          <t>310</t>
+        </is>
       </c>
       <c r="D10">
         <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>330</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
+          <t>Hepatitis a</t>
         </is>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Enfermedades huerfanas - raras</t>
+          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
         </is>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ira por virus nuevo</t>
+          <t>Enfermedades huerfanas - raras</t>
         </is>
       </c>
       <c r="C13">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Infeccion respiratoria aguda grave irag inusitada</t>
+          <t>Ira por virus nuevo</t>
         </is>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
+          <t>Infeccion respiratoria aguda grave irag inusitada</t>
         </is>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>0.37</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
+          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
         </is>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>355</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Intento de suicidio</t>
+          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
         </is>
       </c>
       <c r="C17">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -723,201 +712,201 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>356</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Iad - infecciones asociadas a dispositivos - individual</t>
+          <t>Intento de suicidio</t>
         </is>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <v>0.14</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>357</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Intoxicaciones</t>
+          <t>Iad - infecciones asociadas a dispositivos - individual</t>
         </is>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>0.09</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>365</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Leishmaniasis cutanea</t>
+          <t>Intoxicaciones</t>
         </is>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>420</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Leptospirosis</t>
+          <t>Leishmaniasis cutanea</t>
         </is>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Malaria</t>
+          <t>Leptospirosis</t>
         </is>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>535</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
+          <t>Malaria</t>
         </is>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>535</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Morbilidad materna extrema</t>
+          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
         </is>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>549</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Mortalidad perinatal y neonatal tardia</t>
+          <t>Morbilidad materna extrema</t>
         </is>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>0.37</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>560</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mortalidad por dengue</t>
+          <t>Mortalidad perinatal y neonatal tardia</t>
         </is>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>580</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
+          <t>Mortalidad por dengue</t>
         </is>
       </c>
       <c r="C27">
@@ -933,148 +922,169 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>591</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Parotiditis</t>
+          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
         </is>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>0.27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>740</t>
+          <t>620</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sifilis congenita</t>
+          <t>Parotiditis</t>
         </is>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>750</t>
+          <t>740</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sifilis gestacional</t>
+          <t>Sifilis congenita</t>
         </is>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>750</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tos ferina</t>
+          <t>Sifilis gestacional</t>
         </is>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>813</t>
+          <t>800</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tuberculosis</t>
+          <t>Tos ferina</t>
         </is>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>0.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>831</t>
+          <t>813</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Varicela individual</t>
+          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
         <v>9</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>831</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Varicela individual</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>850</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B35" t="inlineStr">
         <is>
           <t>Vih/sida/mortalidad por sida</t>
         </is>
       </c>
-      <c r="C34">
-        <v>11</v>
-      </c>
-      <c r="D34">
-        <v>8</v>
-      </c>
-      <c r="E34">
-        <v>0.09</v>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
semana 33 de 2025
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -396,13 +396,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -420,10 +420,10 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -441,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>0.18</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6">
@@ -480,13 +480,13 @@
         </is>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7">
@@ -504,10 +504,10 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -543,293 +543,304 @@
         </is>
       </c>
       <c r="C9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D9">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="E9">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>310</t>
-        </is>
+          <t>330</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hepatitis a</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hepatitis a</t>
+          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
         </is>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
+          <t>Enfermedades huerfanas - raras</t>
         </is>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Enfermedades huerfanas - raras</t>
+          <t>Ira por virus nuevo</t>
         </is>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ira por virus nuevo</t>
+          <t>Infeccion respiratoria aguda grave irag inusitada</t>
         </is>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Infeccion respiratoria aguda grave irag inusitada</t>
+          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
         </is>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>355</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
+          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
         </is>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>356</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
+          <t>Intento de suicidio</t>
         </is>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>357</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Intento de suicidio</t>
+          <t>Iad - infecciones asociadas a dispositivos - individual</t>
         </is>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>365</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Iad - infecciones asociadas a dispositivos - individual</t>
+          <t>Intoxicaciones</t>
         </is>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>420</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Intoxicaciones</t>
+          <t>Leishmaniasis cutanea</t>
         </is>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Leishmaniasis cutanea</t>
+          <t>Leptospirosis</t>
         </is>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Leptospirosis</t>
+          <t>Malaria</t>
         </is>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>535</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Malaria</t>
+          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
         </is>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -838,75 +849,75 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>535</t>
+          <t>549</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
+          <t>Morbilidad materna extrema</t>
         </is>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>560</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Morbilidad materna extrema</t>
+          <t>Mortalidad perinatal y neonatal tardia</t>
         </is>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0.2</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>580</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mortalidad perinatal y neonatal tardia</t>
+          <t>Mortalidad por dengue</t>
         </is>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0.37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>591</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Mortalidad por dengue</t>
+          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
         </is>
       </c>
       <c r="C27">
@@ -922,22 +933,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>591</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
-        </is>
-      </c>
-      <c r="C28">
-        <v>0</v>
+          <t>610</t>
+        </is>
       </c>
       <c r="D28">
         <v>0</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -952,13 +952,13 @@
         </is>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="30">
@@ -976,10 +976,10 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -997,10 +997,10 @@
         <v>2</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="32">
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1057,13 +1057,13 @@
         </is>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35">
@@ -1078,13 +1078,13 @@
         </is>
       </c>
       <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
         <v>7</v>
       </c>
-      <c r="D35">
-        <v>5</v>
-      </c>
       <c r="E35">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inicio de año epidemiologico 2026, semana 4 2026
</commit_message>
<xml_diff>
--- a/Boletin_ Epi_Pereira/Datos/poisson.xlsx
+++ b/Boletin_ Epi_Pereira/Datos/poisson.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,40 +387,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>113</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Accidente ofidico</t>
+          <t>Desnutrici”n aguda en menores de 5 anos</t>
         </is>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>115</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Desnutrici”n aguda en menores de 5 anos</t>
+          <t>Cancer en menores de 18 anos</t>
         </is>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0.37</v>
@@ -429,348 +429,348 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>155</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cancer en menores de 18 anos</t>
+          <t>Cancer de la mama y cuello uterino</t>
         </is>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>210</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cancer de la mama y cuello uterino</t>
+          <t>Dengue</t>
         </is>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>215</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dengue</t>
+          <t>Defectos congenitos</t>
         </is>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>215</t>
+          <t>300</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Defectos congenitos</t>
+          <t>Agresiones por animales potencialmente transmisores de rabia</t>
         </is>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>0.17</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>220</t>
+          <t>330</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dengue grave</t>
+          <t>Hepatitis a</t>
         </is>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>340</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Agresiones por animales potencialmente transmisores de rabia</t>
+          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
         </is>
       </c>
       <c r="C9">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>330</t>
+          <t>342</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hepatitis a</t>
+          <t>Enfermedades huerfanas - raras</t>
         </is>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E10">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>340</t>
+          <t>346</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hepatitis b, c y coinfeccion hepatitis b y delta</t>
+          <t>Ira por virus nuevo</t>
         </is>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>294</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Enfermedades huerfanas - raras</t>
+          <t>Infeccion respiratoria aguda grave irag inusitada</t>
         </is>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0.14</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>346</t>
+          <t>352</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ira por virus nuevo</t>
+          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
         </is>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>348</t>
+          <t>355</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Infeccion respiratoria aguda grave irag inusitada</t>
+          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
         </is>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0.14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>352</t>
+          <t>356</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Infecciones de sitio quirurgico asociadas a procedimiento medico quirurgico</t>
+          <t>Intento de suicidio</t>
         </is>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>0.37</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>355</t>
+          <t>357</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Enfermedad transmitida por alimentos o agua (eta)</t>
+          <t>Iad - infecciones asociadas a dispositivos - individual</t>
         </is>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>356</t>
+          <t>365</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Intento de suicidio</t>
+          <t>Intoxicaciones</t>
         </is>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>0.07000000000000001</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>455</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Iad - infecciones asociadas a dispositivos - individual</t>
+          <t>Leptospirosis</t>
         </is>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>365</t>
+          <t>465</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Intoxicaciones</t>
+          <t>Malaria</t>
         </is>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>420</t>
+          <t>535</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Leishmaniasis cutanea</t>
+          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
         </is>
       </c>
       <c r="C20">
@@ -786,33 +786,33 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>549</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lepra</t>
+          <t>Morbilidad materna extrema</t>
         </is>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>455</t>
+          <t>560</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Leptospirosis</t>
+          <t>Mortalidad perinatal y neonatal tardia</t>
         </is>
       </c>
       <c r="C22">
@@ -828,12 +828,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>465</t>
+          <t>580</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Malaria</t>
+          <t>Mortalidad por dengue</t>
         </is>
       </c>
       <c r="C23">
@@ -849,12 +849,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>535</t>
+          <t>591</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Meningitis bacteriana y enfermedad meningoc”cica</t>
+          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
         </is>
       </c>
       <c r="C24">
@@ -870,274 +870,106 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>549</t>
+          <t>750</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Morbilidad materna extrema</t>
+          <t>Sifilis gestacional</t>
         </is>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>560</t>
+          <t>800</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mortalidad perinatal y neonatal tardia</t>
+          <t>Tos ferina</t>
         </is>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>580</t>
+          <t>813</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Mortalidad por dengue</t>
+          <t>Tuberculosis</t>
         </is>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>831</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Vigilancia integrada de muertes en menores de cinco anos por infeccion respiratoria aguda - enfermedad diarreica aguda y/o desnutricion</t>
+          <t>Varicela individual</t>
         </is>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>620</t>
+          <t>850</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Parotiditis</t>
+          <t>Vih/sida/mortalidad por sida</t>
         </is>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>730</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Sarampion</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>740</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Sifilis congenita</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>750</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Sifilis gestacional</t>
-        </is>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Tos ferina</t>
-        </is>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>813</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Tuberculosis</t>
-        </is>
-      </c>
-      <c r="C34">
-        <v>6</v>
-      </c>
-      <c r="D34">
-        <v>6</v>
-      </c>
-      <c r="E34">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>831</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Varicela individual</t>
-        </is>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>0.07000000000000001</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>850</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Vih/sida/mortalidad por sida</t>
-        </is>
-      </c>
-      <c r="C36">
-        <v>8</v>
-      </c>
-      <c r="D36">
-        <v>11</v>
-      </c>
-      <c r="E36">
-        <v>0.07000000000000001</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>895</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Zika</t>
-        </is>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>